<commit_message>
commit before report on test for property
</commit_message>
<xml_diff>
--- a/dataset/property-experiment/sequence/resutl-on-01_log_sequence_02.xlsx
+++ b/dataset/property-experiment/sequence/resutl-on-01_log_sequence_02.xlsx
@@ -163,7 +163,7 @@
         <v>0.05</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M2" t="n">
         <v>0.1</v>
@@ -204,7 +204,7 @@
         <v>0.1</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M3" t="n">
         <v>0.1</v>
@@ -245,7 +245,7 @@
         <v>0.2</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M4" t="n">
         <v>0.1</v>
@@ -286,7 +286,7 @@
         <v>0.3</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M5" t="n">
         <v>0.1</v>
@@ -327,7 +327,7 @@
         <v>0.4</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M6" t="n">
         <v>0.1</v>
@@ -368,7 +368,7 @@
         <v>0.5</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M7" t="n">
         <v>0.1</v>
@@ -409,7 +409,7 @@
         <v>0.6</v>
       </c>
       <c r="L8" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M8" t="n">
         <v>0.1</v>
@@ -450,7 +450,7 @@
         <v>0.7</v>
       </c>
       <c r="L9" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M9" t="n">
         <v>0.1</v>
@@ -491,7 +491,7 @@
         <v>0.8</v>
       </c>
       <c r="L10" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M10" t="n">
         <v>0.1</v>
@@ -532,7 +532,7 @@
         <v>0.9</v>
       </c>
       <c r="L11" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M11" t="n">
         <v>0.1</v>
@@ -573,7 +573,7 @@
         <v>1.0</v>
       </c>
       <c r="L12" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="M12" t="n">
         <v>0.1</v>
@@ -614,7 +614,7 @@
         <v>0.05</v>
       </c>
       <c r="L13" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M13" t="n">
         <v>0.3</v>
@@ -655,7 +655,7 @@
         <v>0.1</v>
       </c>
       <c r="L14" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M14" t="n">
         <v>0.3</v>
@@ -696,7 +696,7 @@
         <v>0.2</v>
       </c>
       <c r="L15" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M15" t="n">
         <v>0.3</v>
@@ -737,7 +737,7 @@
         <v>0.3</v>
       </c>
       <c r="L16" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M16" t="n">
         <v>0.3</v>
@@ -778,7 +778,7 @@
         <v>0.4</v>
       </c>
       <c r="L17" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M17" t="n">
         <v>0.3</v>
@@ -819,7 +819,7 @@
         <v>0.5</v>
       </c>
       <c r="L18" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M18" t="n">
         <v>0.3</v>
@@ -860,7 +860,7 @@
         <v>0.6</v>
       </c>
       <c r="L19" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M19" t="n">
         <v>0.3</v>
@@ -901,7 +901,7 @@
         <v>0.7</v>
       </c>
       <c r="L20" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M20" t="n">
         <v>0.3</v>
@@ -942,7 +942,7 @@
         <v>0.8</v>
       </c>
       <c r="L21" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M21" t="n">
         <v>0.3</v>
@@ -983,7 +983,7 @@
         <v>0.9</v>
       </c>
       <c r="L22" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M22" t="n">
         <v>0.3</v>
@@ -1024,7 +1024,7 @@
         <v>1.0</v>
       </c>
       <c r="L23" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="M23" t="n">
         <v>0.3</v>
@@ -1065,7 +1065,7 @@
         <v>0.05</v>
       </c>
       <c r="L24" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M24" t="n">
         <v>0.5</v>
@@ -1106,7 +1106,7 @@
         <v>0.1</v>
       </c>
       <c r="L25" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M25" t="n">
         <v>0.5</v>
@@ -1147,7 +1147,7 @@
         <v>0.2</v>
       </c>
       <c r="L26" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M26" t="n">
         <v>0.5</v>
@@ -1188,7 +1188,7 @@
         <v>0.3</v>
       </c>
       <c r="L27" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M27" t="n">
         <v>0.5</v>
@@ -1229,7 +1229,7 @@
         <v>0.4</v>
       </c>
       <c r="L28" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M28" t="n">
         <v>0.5</v>
@@ -1270,7 +1270,7 @@
         <v>0.5</v>
       </c>
       <c r="L29" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M29" t="n">
         <v>0.5</v>
@@ -1311,7 +1311,7 @@
         <v>0.6</v>
       </c>
       <c r="L30" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M30" t="n">
         <v>0.5</v>
@@ -1352,7 +1352,7 @@
         <v>0.7</v>
       </c>
       <c r="L31" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M31" t="n">
         <v>0.5</v>
@@ -1393,7 +1393,7 @@
         <v>0.8</v>
       </c>
       <c r="L32" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M32" t="n">
         <v>0.5</v>
@@ -1434,7 +1434,7 @@
         <v>0.9</v>
       </c>
       <c r="L33" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M33" t="n">
         <v>0.5</v>
@@ -1475,7 +1475,7 @@
         <v>1.0</v>
       </c>
       <c r="L34" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="M34" t="n">
         <v>0.5</v>
@@ -1516,7 +1516,7 @@
         <v>0.05</v>
       </c>
       <c r="L35" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M35" t="n">
         <v>0.7</v>
@@ -1557,7 +1557,7 @@
         <v>0.1</v>
       </c>
       <c r="L36" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M36" t="n">
         <v>0.7</v>
@@ -1598,7 +1598,7 @@
         <v>0.2</v>
       </c>
       <c r="L37" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M37" t="n">
         <v>0.7</v>
@@ -1639,7 +1639,7 @@
         <v>0.3</v>
       </c>
       <c r="L38" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M38" t="n">
         <v>0.7</v>
@@ -1680,7 +1680,7 @@
         <v>0.4</v>
       </c>
       <c r="L39" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M39" t="n">
         <v>0.7</v>
@@ -1721,7 +1721,7 @@
         <v>0.5</v>
       </c>
       <c r="L40" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M40" t="n">
         <v>0.7</v>
@@ -1762,7 +1762,7 @@
         <v>0.6</v>
       </c>
       <c r="L41" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M41" t="n">
         <v>0.7</v>
@@ -1803,7 +1803,7 @@
         <v>0.7</v>
       </c>
       <c r="L42" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M42" t="n">
         <v>0.7</v>
@@ -1844,7 +1844,7 @@
         <v>0.8</v>
       </c>
       <c r="L43" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M43" t="n">
         <v>0.7</v>
@@ -1885,7 +1885,7 @@
         <v>0.9</v>
       </c>
       <c r="L44" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M44" t="n">
         <v>0.7</v>
@@ -1926,7 +1926,7 @@
         <v>1.0</v>
       </c>
       <c r="L45" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="M45" t="n">
         <v>0.7</v>
@@ -1967,7 +1967,7 @@
         <v>0.05</v>
       </c>
       <c r="L46" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M46" t="n">
         <v>1.0</v>
@@ -2008,7 +2008,7 @@
         <v>0.1</v>
       </c>
       <c r="L47" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M47" t="n">
         <v>1.0</v>
@@ -2049,7 +2049,7 @@
         <v>0.2</v>
       </c>
       <c r="L48" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M48" t="n">
         <v>1.0</v>
@@ -2090,7 +2090,7 @@
         <v>0.3</v>
       </c>
       <c r="L49" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M49" t="n">
         <v>1.0</v>
@@ -2131,7 +2131,7 @@
         <v>0.4</v>
       </c>
       <c r="L50" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M50" t="n">
         <v>1.0</v>
@@ -2172,7 +2172,7 @@
         <v>0.5</v>
       </c>
       <c r="L51" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M51" t="n">
         <v>1.0</v>
@@ -2213,7 +2213,7 @@
         <v>0.6</v>
       </c>
       <c r="L52" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M52" t="n">
         <v>1.0</v>
@@ -2254,7 +2254,7 @@
         <v>0.7</v>
       </c>
       <c r="L53" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M53" t="n">
         <v>1.0</v>
@@ -2295,7 +2295,7 @@
         <v>0.8</v>
       </c>
       <c r="L54" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M54" t="n">
         <v>1.0</v>
@@ -2336,7 +2336,7 @@
         <v>0.9</v>
       </c>
       <c r="L55" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M55" t="n">
         <v>1.0</v>
@@ -2377,7 +2377,7 @@
         <v>1.0</v>
       </c>
       <c r="L56" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="M56" t="n">
         <v>1.0</v>
@@ -2388,10 +2388,10 @@
         <v>50.0</v>
       </c>
       <c r="B57" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C57" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D57" t="n">
         <v>0.0</v>
@@ -2400,22 +2400,22 @@
         <v>1.0</v>
       </c>
       <c r="F57" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G57" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H57" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I57" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J57" t="n">
         <v>1.0</v>
       </c>
       <c r="K57" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L57" t="n">
         <v>0.05</v>
@@ -2429,10 +2429,10 @@
         <v>50.0</v>
       </c>
       <c r="B58" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C58" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D58" t="n">
         <v>0.0</v>
@@ -2441,22 +2441,22 @@
         <v>1.0</v>
       </c>
       <c r="F58" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G58" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H58" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I58" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J58" t="n">
         <v>1.0</v>
       </c>
       <c r="K58" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L58" t="n">
         <v>0.1</v>
@@ -2470,10 +2470,10 @@
         <v>50.0</v>
       </c>
       <c r="B59" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C59" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D59" t="n">
         <v>0.0</v>
@@ -2482,22 +2482,22 @@
         <v>1.0</v>
       </c>
       <c r="F59" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G59" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H59" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I59" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J59" t="n">
         <v>1.0</v>
       </c>
       <c r="K59" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L59" t="n">
         <v>0.2</v>
@@ -2511,10 +2511,10 @@
         <v>50.0</v>
       </c>
       <c r="B60" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C60" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D60" t="n">
         <v>0.0</v>
@@ -2523,22 +2523,22 @@
         <v>1.0</v>
       </c>
       <c r="F60" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G60" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H60" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I60" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J60" t="n">
         <v>1.0</v>
       </c>
       <c r="K60" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L60" t="n">
         <v>0.3</v>
@@ -2552,10 +2552,10 @@
         <v>50.0</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C61" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D61" t="n">
         <v>0.0</v>
@@ -2564,22 +2564,22 @@
         <v>1.0</v>
       </c>
       <c r="F61" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G61" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H61" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I61" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J61" t="n">
         <v>1.0</v>
       </c>
       <c r="K61" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L61" t="n">
         <v>0.4</v>
@@ -2593,10 +2593,10 @@
         <v>50.0</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C62" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D62" t="n">
         <v>0.0</v>
@@ -2605,22 +2605,22 @@
         <v>1.0</v>
       </c>
       <c r="F62" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G62" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H62" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I62" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J62" t="n">
         <v>1.0</v>
       </c>
       <c r="K62" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L62" t="n">
         <v>0.5</v>
@@ -2634,10 +2634,10 @@
         <v>50.0</v>
       </c>
       <c r="B63" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C63" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D63" t="n">
         <v>0.0</v>
@@ -2646,22 +2646,22 @@
         <v>1.0</v>
       </c>
       <c r="F63" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G63" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H63" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I63" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J63" t="n">
         <v>1.0</v>
       </c>
       <c r="K63" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L63" t="n">
         <v>0.6</v>
@@ -2675,10 +2675,10 @@
         <v>50.0</v>
       </c>
       <c r="B64" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C64" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D64" t="n">
         <v>0.0</v>
@@ -2687,22 +2687,22 @@
         <v>1.0</v>
       </c>
       <c r="F64" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G64" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H64" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I64" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J64" t="n">
         <v>1.0</v>
       </c>
       <c r="K64" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L64" t="n">
         <v>0.7</v>
@@ -2716,10 +2716,10 @@
         <v>50.0</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C65" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D65" t="n">
         <v>0.0</v>
@@ -2728,22 +2728,22 @@
         <v>1.0</v>
       </c>
       <c r="F65" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G65" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H65" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I65" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J65" t="n">
         <v>1.0</v>
       </c>
       <c r="K65" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L65" t="n">
         <v>0.8</v>
@@ -2757,10 +2757,10 @@
         <v>50.0</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C66" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D66" t="n">
         <v>0.0</v>
@@ -2769,22 +2769,22 @@
         <v>1.0</v>
       </c>
       <c r="F66" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G66" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H66" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I66" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J66" t="n">
         <v>1.0</v>
       </c>
       <c r="K66" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L66" t="n">
         <v>0.9</v>
@@ -2798,10 +2798,10 @@
         <v>50.0</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C67" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D67" t="n">
         <v>0.0</v>
@@ -2810,22 +2810,22 @@
         <v>1.0</v>
       </c>
       <c r="F67" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G67" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H67" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I67" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J67" t="n">
         <v>1.0</v>
       </c>
       <c r="K67" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L67" t="n">
         <v>1.0</v>
@@ -2866,7 +2866,7 @@
         <v>2.0</v>
       </c>
       <c r="K68" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L68" t="n">
         <v>0.05</v>
@@ -2907,7 +2907,7 @@
         <v>2.0</v>
       </c>
       <c r="K69" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L69" t="n">
         <v>0.1</v>
@@ -2948,7 +2948,7 @@
         <v>2.0</v>
       </c>
       <c r="K70" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L70" t="n">
         <v>0.2</v>
@@ -2989,7 +2989,7 @@
         <v>2.0</v>
       </c>
       <c r="K71" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L71" t="n">
         <v>0.3</v>
@@ -3030,7 +3030,7 @@
         <v>2.0</v>
       </c>
       <c r="K72" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L72" t="n">
         <v>0.4</v>
@@ -3071,7 +3071,7 @@
         <v>2.0</v>
       </c>
       <c r="K73" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L73" t="n">
         <v>0.5</v>
@@ -3112,7 +3112,7 @@
         <v>2.0</v>
       </c>
       <c r="K74" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L74" t="n">
         <v>0.6</v>
@@ -3153,7 +3153,7 @@
         <v>2.0</v>
       </c>
       <c r="K75" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L75" t="n">
         <v>0.7</v>
@@ -3194,7 +3194,7 @@
         <v>2.0</v>
       </c>
       <c r="K76" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L76" t="n">
         <v>0.8</v>
@@ -3235,7 +3235,7 @@
         <v>2.0</v>
       </c>
       <c r="K77" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L77" t="n">
         <v>0.9</v>
@@ -3276,7 +3276,7 @@
         <v>2.0</v>
       </c>
       <c r="K78" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L78" t="n">
         <v>1.0</v>
@@ -3290,10 +3290,10 @@
         <v>50.0</v>
       </c>
       <c r="B79" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C79" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D79" t="n">
         <v>0.0</v>
@@ -3302,22 +3302,22 @@
         <v>1.0</v>
       </c>
       <c r="F79" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G79" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H79" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I79" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J79" t="n">
         <v>3.0</v>
       </c>
       <c r="K79" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L79" t="n">
         <v>0.05</v>
@@ -3331,10 +3331,10 @@
         <v>50.0</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C80" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D80" t="n">
         <v>0.0</v>
@@ -3343,22 +3343,22 @@
         <v>1.0</v>
       </c>
       <c r="F80" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G80" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H80" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I80" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J80" t="n">
         <v>3.0</v>
       </c>
       <c r="K80" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L80" t="n">
         <v>0.1</v>
@@ -3372,10 +3372,10 @@
         <v>50.0</v>
       </c>
       <c r="B81" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C81" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D81" t="n">
         <v>0.0</v>
@@ -3384,22 +3384,22 @@
         <v>1.0</v>
       </c>
       <c r="F81" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G81" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H81" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I81" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J81" t="n">
         <v>3.0</v>
       </c>
       <c r="K81" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L81" t="n">
         <v>0.2</v>
@@ -3413,10 +3413,10 @@
         <v>50.0</v>
       </c>
       <c r="B82" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C82" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D82" t="n">
         <v>0.0</v>
@@ -3425,22 +3425,22 @@
         <v>1.0</v>
       </c>
       <c r="F82" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G82" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H82" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I82" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J82" t="n">
         <v>3.0</v>
       </c>
       <c r="K82" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L82" t="n">
         <v>0.3</v>
@@ -3454,10 +3454,10 @@
         <v>50.0</v>
       </c>
       <c r="B83" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C83" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D83" t="n">
         <v>0.0</v>
@@ -3466,22 +3466,22 @@
         <v>1.0</v>
       </c>
       <c r="F83" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G83" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H83" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I83" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J83" t="n">
         <v>3.0</v>
       </c>
       <c r="K83" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L83" t="n">
         <v>0.4</v>
@@ -3495,10 +3495,10 @@
         <v>50.0</v>
       </c>
       <c r="B84" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C84" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D84" t="n">
         <v>0.0</v>
@@ -3507,22 +3507,22 @@
         <v>1.0</v>
       </c>
       <c r="F84" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G84" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H84" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I84" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J84" t="n">
         <v>3.0</v>
       </c>
       <c r="K84" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L84" t="n">
         <v>0.5</v>
@@ -3536,10 +3536,10 @@
         <v>50.0</v>
       </c>
       <c r="B85" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C85" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D85" t="n">
         <v>0.0</v>
@@ -3548,22 +3548,22 @@
         <v>1.0</v>
       </c>
       <c r="F85" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G85" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H85" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I85" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J85" t="n">
         <v>3.0</v>
       </c>
       <c r="K85" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L85" t="n">
         <v>0.6</v>
@@ -3577,10 +3577,10 @@
         <v>50.0</v>
       </c>
       <c r="B86" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C86" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D86" t="n">
         <v>0.0</v>
@@ -3589,22 +3589,22 @@
         <v>1.0</v>
       </c>
       <c r="F86" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G86" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H86" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I86" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J86" t="n">
         <v>3.0</v>
       </c>
       <c r="K86" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L86" t="n">
         <v>0.7</v>
@@ -3618,10 +3618,10 @@
         <v>50.0</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C87" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D87" t="n">
         <v>0.0</v>
@@ -3630,22 +3630,22 @@
         <v>1.0</v>
       </c>
       <c r="F87" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G87" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H87" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I87" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J87" t="n">
         <v>3.0</v>
       </c>
       <c r="K87" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L87" t="n">
         <v>0.8</v>
@@ -3659,10 +3659,10 @@
         <v>50.0</v>
       </c>
       <c r="B88" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C88" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D88" t="n">
         <v>0.0</v>
@@ -3671,22 +3671,22 @@
         <v>1.0</v>
       </c>
       <c r="F88" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G88" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H88" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I88" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J88" t="n">
         <v>3.0</v>
       </c>
       <c r="K88" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L88" t="n">
         <v>0.9</v>
@@ -3700,10 +3700,10 @@
         <v>50.0</v>
       </c>
       <c r="B89" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C89" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D89" t="n">
         <v>0.0</v>
@@ -3712,22 +3712,22 @@
         <v>1.0</v>
       </c>
       <c r="F89" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G89" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H89" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I89" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J89" t="n">
         <v>3.0</v>
       </c>
       <c r="K89" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L89" t="n">
         <v>1.0</v>
@@ -3768,7 +3768,7 @@
         <v>4.0</v>
       </c>
       <c r="K90" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L90" t="n">
         <v>0.05</v>
@@ -3809,7 +3809,7 @@
         <v>4.0</v>
       </c>
       <c r="K91" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L91" t="n">
         <v>0.1</v>
@@ -3850,7 +3850,7 @@
         <v>4.0</v>
       </c>
       <c r="K92" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L92" t="n">
         <v>0.2</v>
@@ -3891,7 +3891,7 @@
         <v>4.0</v>
       </c>
       <c r="K93" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L93" t="n">
         <v>0.3</v>
@@ -3932,7 +3932,7 @@
         <v>4.0</v>
       </c>
       <c r="K94" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L94" t="n">
         <v>0.4</v>
@@ -3973,7 +3973,7 @@
         <v>4.0</v>
       </c>
       <c r="K95" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L95" t="n">
         <v>0.5</v>
@@ -4014,7 +4014,7 @@
         <v>4.0</v>
       </c>
       <c r="K96" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L96" t="n">
         <v>0.6</v>
@@ -4055,7 +4055,7 @@
         <v>4.0</v>
       </c>
       <c r="K97" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L97" t="n">
         <v>0.7</v>
@@ -4096,7 +4096,7 @@
         <v>4.0</v>
       </c>
       <c r="K98" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L98" t="n">
         <v>0.8</v>
@@ -4137,7 +4137,7 @@
         <v>4.0</v>
       </c>
       <c r="K99" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L99" t="n">
         <v>0.9</v>
@@ -4178,7 +4178,7 @@
         <v>4.0</v>
       </c>
       <c r="K100" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L100" t="n">
         <v>1.0</v>
@@ -4219,7 +4219,7 @@
         <v>5.0</v>
       </c>
       <c r="K101" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L101" t="n">
         <v>0.05</v>
@@ -4260,7 +4260,7 @@
         <v>5.0</v>
       </c>
       <c r="K102" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L102" t="n">
         <v>0.1</v>
@@ -4301,7 +4301,7 @@
         <v>5.0</v>
       </c>
       <c r="K103" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L103" t="n">
         <v>0.2</v>
@@ -4342,7 +4342,7 @@
         <v>5.0</v>
       </c>
       <c r="K104" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L104" t="n">
         <v>0.3</v>
@@ -4383,7 +4383,7 @@
         <v>5.0</v>
       </c>
       <c r="K105" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L105" t="n">
         <v>0.4</v>
@@ -4424,7 +4424,7 @@
         <v>5.0</v>
       </c>
       <c r="K106" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L106" t="n">
         <v>0.5</v>
@@ -4465,7 +4465,7 @@
         <v>5.0</v>
       </c>
       <c r="K107" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L107" t="n">
         <v>0.6</v>
@@ -4506,7 +4506,7 @@
         <v>5.0</v>
       </c>
       <c r="K108" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L108" t="n">
         <v>0.7</v>
@@ -4547,7 +4547,7 @@
         <v>5.0</v>
       </c>
       <c r="K109" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L109" t="n">
         <v>0.8</v>
@@ -4588,7 +4588,7 @@
         <v>5.0</v>
       </c>
       <c r="K110" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L110" t="n">
         <v>0.9</v>
@@ -4629,7 +4629,7 @@
         <v>5.0</v>
       </c>
       <c r="K111" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L111" t="n">
         <v>1.0</v>
@@ -4670,7 +4670,7 @@
         <v>1.0</v>
       </c>
       <c r="K112" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L112" t="n">
         <v>0.1</v>
@@ -4684,10 +4684,10 @@
         <v>50.0</v>
       </c>
       <c r="B113" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C113" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D113" t="n">
         <v>0.0</v>
@@ -4696,22 +4696,22 @@
         <v>1.0</v>
       </c>
       <c r="F113" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G113" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H113" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I113" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J113" t="n">
         <v>1.0</v>
       </c>
       <c r="K113" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L113" t="n">
         <v>0.1</v>
@@ -4752,7 +4752,7 @@
         <v>1.0</v>
       </c>
       <c r="K114" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L114" t="n">
         <v>0.1</v>
@@ -4793,7 +4793,7 @@
         <v>1.0</v>
       </c>
       <c r="K115" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L115" t="n">
         <v>0.1</v>
@@ -4834,7 +4834,7 @@
         <v>1.0</v>
       </c>
       <c r="K116" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L116" t="n">
         <v>0.1</v>
@@ -4875,7 +4875,7 @@
         <v>1.0</v>
       </c>
       <c r="K117" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L117" t="n">
         <v>0.1</v>
@@ -4916,7 +4916,7 @@
         <v>1.0</v>
       </c>
       <c r="K118" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L118" t="n">
         <v>0.1</v>
@@ -4957,7 +4957,7 @@
         <v>1.0</v>
       </c>
       <c r="K119" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L119" t="n">
         <v>0.1</v>
@@ -4998,7 +4998,7 @@
         <v>1.0</v>
       </c>
       <c r="K120" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L120" t="n">
         <v>0.1</v>
@@ -5039,7 +5039,7 @@
         <v>1.0</v>
       </c>
       <c r="K121" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L121" t="n">
         <v>0.1</v>
@@ -5080,7 +5080,7 @@
         <v>1.0</v>
       </c>
       <c r="K122" t="n">
-        <v>0.1</v>
+        <v>0.12277500812053187</v>
       </c>
       <c r="L122" t="n">
         <v>0.1</v>
@@ -5121,7 +5121,7 @@
         <v>2.0</v>
       </c>
       <c r="K123" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L123" t="n">
         <v>0.3</v>
@@ -5162,7 +5162,7 @@
         <v>2.0</v>
       </c>
       <c r="K124" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L124" t="n">
         <v>0.3</v>
@@ -5203,7 +5203,7 @@
         <v>2.0</v>
       </c>
       <c r="K125" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L125" t="n">
         <v>0.3</v>
@@ -5244,7 +5244,7 @@
         <v>2.0</v>
       </c>
       <c r="K126" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L126" t="n">
         <v>0.3</v>
@@ -5285,7 +5285,7 @@
         <v>2.0</v>
       </c>
       <c r="K127" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L127" t="n">
         <v>0.3</v>
@@ -5326,7 +5326,7 @@
         <v>2.0</v>
       </c>
       <c r="K128" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L128" t="n">
         <v>0.3</v>
@@ -5367,7 +5367,7 @@
         <v>2.0</v>
       </c>
       <c r="K129" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L129" t="n">
         <v>0.3</v>
@@ -5408,7 +5408,7 @@
         <v>2.0</v>
       </c>
       <c r="K130" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L130" t="n">
         <v>0.3</v>
@@ -5449,7 +5449,7 @@
         <v>2.0</v>
       </c>
       <c r="K131" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L131" t="n">
         <v>0.3</v>
@@ -5490,7 +5490,7 @@
         <v>2.0</v>
       </c>
       <c r="K132" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L132" t="n">
         <v>0.3</v>
@@ -5531,7 +5531,7 @@
         <v>2.0</v>
       </c>
       <c r="K133" t="n">
-        <v>0.3</v>
+        <v>0.23622398660555474</v>
       </c>
       <c r="L133" t="n">
         <v>0.3</v>
@@ -5572,7 +5572,7 @@
         <v>3.0</v>
       </c>
       <c r="K134" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L134" t="n">
         <v>0.5</v>
@@ -5613,7 +5613,7 @@
         <v>3.0</v>
       </c>
       <c r="K135" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L135" t="n">
         <v>0.5</v>
@@ -5654,7 +5654,7 @@
         <v>3.0</v>
       </c>
       <c r="K136" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L136" t="n">
         <v>0.5</v>
@@ -5695,7 +5695,7 @@
         <v>3.0</v>
       </c>
       <c r="K137" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L137" t="n">
         <v>0.5</v>
@@ -5736,7 +5736,7 @@
         <v>3.0</v>
       </c>
       <c r="K138" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L138" t="n">
         <v>0.5</v>
@@ -5750,10 +5750,10 @@
         <v>50.0</v>
       </c>
       <c r="B139" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="C139" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D139" t="n">
         <v>0.0</v>
@@ -5762,22 +5762,22 @@
         <v>1.0</v>
       </c>
       <c r="F139" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="G139" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="H139" t="n">
-        <v>1.0</v>
+        <v>0.5</v>
       </c>
       <c r="I139" t="n">
-        <v>1.0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="J139" t="n">
         <v>3.0</v>
       </c>
       <c r="K139" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L139" t="n">
         <v>0.5</v>
@@ -5818,7 +5818,7 @@
         <v>3.0</v>
       </c>
       <c r="K140" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L140" t="n">
         <v>0.5</v>
@@ -5859,7 +5859,7 @@
         <v>3.0</v>
       </c>
       <c r="K141" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L141" t="n">
         <v>0.5</v>
@@ -5900,7 +5900,7 @@
         <v>3.0</v>
       </c>
       <c r="K142" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L142" t="n">
         <v>0.5</v>
@@ -5941,7 +5941,7 @@
         <v>3.0</v>
       </c>
       <c r="K143" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L143" t="n">
         <v>0.5</v>
@@ -5982,7 +5982,7 @@
         <v>3.0</v>
       </c>
       <c r="K144" t="n">
-        <v>0.5</v>
+        <v>0.5519964298249218</v>
       </c>
       <c r="L144" t="n">
         <v>0.5</v>
@@ -6023,7 +6023,7 @@
         <v>4.0</v>
       </c>
       <c r="K145" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L145" t="n">
         <v>0.7</v>
@@ -6064,7 +6064,7 @@
         <v>4.0</v>
       </c>
       <c r="K146" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L146" t="n">
         <v>0.7</v>
@@ -6105,7 +6105,7 @@
         <v>4.0</v>
       </c>
       <c r="K147" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L147" t="n">
         <v>0.7</v>
@@ -6146,7 +6146,7 @@
         <v>4.0</v>
       </c>
       <c r="K148" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L148" t="n">
         <v>0.7</v>
@@ -6187,7 +6187,7 @@
         <v>4.0</v>
       </c>
       <c r="K149" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L149" t="n">
         <v>0.7</v>
@@ -6201,10 +6201,10 @@
         <v>50.0</v>
       </c>
       <c r="B150" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="C150" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="D150" t="n">
         <v>0.0</v>
@@ -6213,22 +6213,22 @@
         <v>1.0</v>
       </c>
       <c r="F150" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="G150" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H150" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="I150" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="J150" t="n">
         <v>4.0</v>
       </c>
       <c r="K150" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L150" t="n">
         <v>0.7</v>
@@ -6242,10 +6242,10 @@
         <v>50.0</v>
       </c>
       <c r="B151" t="n">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="C151" t="n">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="D151" t="n">
         <v>0.0</v>
@@ -6254,22 +6254,22 @@
         <v>1.0</v>
       </c>
       <c r="F151" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="G151" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H151" t="n">
-        <v>0.5</v>
+        <v>1.0</v>
       </c>
       <c r="I151" t="n">
-        <v>0.6666666666666666</v>
+        <v>1.0</v>
       </c>
       <c r="J151" t="n">
         <v>4.0</v>
       </c>
       <c r="K151" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L151" t="n">
         <v>0.7</v>
@@ -6310,7 +6310,7 @@
         <v>4.0</v>
       </c>
       <c r="K152" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L152" t="n">
         <v>0.7</v>
@@ -6351,7 +6351,7 @@
         <v>4.0</v>
       </c>
       <c r="K153" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L153" t="n">
         <v>0.7</v>
@@ -6392,7 +6392,7 @@
         <v>4.0</v>
       </c>
       <c r="K154" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L154" t="n">
         <v>0.7</v>
@@ -6433,7 +6433,7 @@
         <v>4.0</v>
       </c>
       <c r="K155" t="n">
-        <v>0.7</v>
+        <v>0.4613099861065403</v>
       </c>
       <c r="L155" t="n">
         <v>0.7</v>
@@ -6474,7 +6474,7 @@
         <v>5.0</v>
       </c>
       <c r="K156" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L156" t="n">
         <v>1.0</v>
@@ -6515,7 +6515,7 @@
         <v>5.0</v>
       </c>
       <c r="K157" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L157" t="n">
         <v>1.0</v>
@@ -6556,7 +6556,7 @@
         <v>5.0</v>
       </c>
       <c r="K158" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L158" t="n">
         <v>1.0</v>
@@ -6597,7 +6597,7 @@
         <v>5.0</v>
       </c>
       <c r="K159" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L159" t="n">
         <v>1.0</v>
@@ -6638,7 +6638,7 @@
         <v>5.0</v>
       </c>
       <c r="K160" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L160" t="n">
         <v>1.0</v>
@@ -6679,7 +6679,7 @@
         <v>5.0</v>
       </c>
       <c r="K161" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L161" t="n">
         <v>1.0</v>
@@ -6720,7 +6720,7 @@
         <v>5.0</v>
       </c>
       <c r="K162" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L162" t="n">
         <v>1.0</v>
@@ -6761,7 +6761,7 @@
         <v>5.0</v>
       </c>
       <c r="K163" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L163" t="n">
         <v>1.0</v>
@@ -6802,7 +6802,7 @@
         <v>5.0</v>
       </c>
       <c r="K164" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L164" t="n">
         <v>1.0</v>
@@ -6843,7 +6843,7 @@
         <v>5.0</v>
       </c>
       <c r="K165" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L165" t="n">
         <v>1.0</v>
@@ -6884,7 +6884,7 @@
         <v>5.0</v>
       </c>
       <c r="K166" t="n">
-        <v>1.0</v>
+        <v>0.9424451812765389</v>
       </c>
       <c r="L166" t="n">
         <v>1.0</v>

</xml_diff>